<commit_message>
working with 2 cucumber steps @Given and @When
</commit_message>
<xml_diff>
--- a/userCredentials.xlsx
+++ b/userCredentials.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\furka\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\furka\IdeaProjects\JiraTasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D6CBBBB-CC69-422D-82A2-B2DC7D029864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E30529-8DDC-4421-A1A2-0A1A6C3E2FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5820" yWindow="-14250" windowWidth="21600" windowHeight="11835" xr2:uid="{037885F4-54E2-4C7B-AE04-E8594EDBD1DD}"/>
+    <workbookView xWindow="28680" yWindow="-9915" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{037885F4-54E2-4C7B-AE04-E8594EDBD1DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Human Resources" sheetId="1" r:id="rId1"/>
@@ -512,13 +512,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB8CDEC5-DE1E-4A53-B828-A4458F32AFE9}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
   </cols>
   <sheetData>
@@ -617,6 +617,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -707,11 +710,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B4AFAC-F805-4F64-B3C9-379F42E77A6B}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
finished; no Assertions no @Then
</commit_message>
<xml_diff>
--- a/userCredentials.xlsx
+++ b/userCredentials.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\furka\IdeaProjects\JiraTasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C49155-E235-4EB8-BC8B-5294C5992557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1226F221-2488-42E8-829E-86AFB51E6EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-9915" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{037885F4-54E2-4C7B-AE04-E8594EDBD1DD}"/>
+    <workbookView xWindow="28680" yWindow="-9915" windowWidth="29040" windowHeight="16440" xr2:uid="{037885F4-54E2-4C7B-AE04-E8594EDBD1DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Human Resources" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="32">
   <si>
     <t>User Name</t>
   </si>
@@ -131,12 +131,16 @@
   </si>
   <si>
     <t>Result</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -161,7 +165,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,6 +176,16 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF4F5F7"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightTrellis">
+        <bgColor indexed="11"/>
       </patternFill>
     </fill>
   </fills>
@@ -202,12 +216,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -524,14 +547,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB8CDEC5-DE1E-4A53-B828-A4458F32AFE9}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" customWidth="1"/>
-    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="32.42578125"/>
+    <col min="2" max="2" customWidth="true" width="19.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -541,9 +564,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -552,6 +573,9 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C2" t="s" s="0">
+        <v>31</v>
+      </c>
     </row>
     <row r="3" spans="1:3" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -560,6 +584,9 @@
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C3" t="s" s="0">
+        <v>31</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -568,6 +595,9 @@
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C4" t="s" s="0">
+        <v>31</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -576,6 +606,9 @@
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C5" t="s" s="0">
+        <v>31</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -584,6 +617,9 @@
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C6" t="s" s="0">
+        <v>31</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -592,6 +628,9 @@
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C7" t="s" s="0">
+        <v>31</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -600,6 +639,9 @@
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C8" t="s" s="0">
+        <v>31</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
@@ -608,6 +650,9 @@
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C9" t="s" s="0">
+        <v>31</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -615,6 +660,9 @@
       </c>
       <c r="B10" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -633,7 +681,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="36.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -728,14 +776,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B4AFAC-F805-4F64-B3C9-379F42E77A6B}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="35.0"/>
+    <col min="2" max="2" customWidth="true" width="14.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>